<commit_message>
fix bulanan tanggal bayar
</commit_message>
<xml_diff>
--- a/server/src/public/bulanan.xlsx
+++ b/server/src/public/bulanan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>siswa_nama</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>lunas</t>
+  </si>
+  <si>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>2022-01-13</t>
+  </si>
+  <si>
+    <t>2022-01-14</t>
   </si>
 </sst>
 </file>
@@ -120,7 +129,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yy/mm/dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -164,7 +173,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -493,7 +502,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,8 +603,8 @@
       <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="4">
-        <v>44636</v>
+      <c r="M2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="N2" t="s">
         <v>16</v>
@@ -638,8 +647,8 @@
       <c r="L3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="4">
-        <v>44637</v>
+      <c r="M3" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="N3" t="s">
         <v>29</v>
@@ -682,8 +691,8 @@
       <c r="L4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="4">
-        <v>44638</v>
+      <c r="M4" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="N4" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Update import data pembayaran bulanan
</commit_message>
<xml_diff>
--- a/server/src/public/bulanan.xlsx
+++ b/server/src/public/bulanan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafly/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD0300E-9C42-C44C-8443-52CA37AAE7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D471C98D-E180-2440-A9E9-6EFBA3D8FA46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,19 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
Update & Fix Error
</commit_message>
<xml_diff>
--- a/server/src/public/bulanan.xlsx
+++ b/server/src/public/bulanan.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\otwku\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafly/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF781CEC-0CFE-45C6-AC9F-2C445526F53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE37110-47C2-6242-A559-BA9126D64E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>siswa_nama</t>
   </si>
@@ -60,15 +72,9 @@
     <t>nama_admin</t>
   </si>
   <si>
-    <t>XII</t>
-  </si>
-  <si>
     <t>RPL</t>
   </si>
   <si>
-    <t>spp</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -84,46 +90,43 @@
     <t>Lunas</t>
   </si>
   <si>
-    <t>spp-124</t>
-  </si>
-  <si>
     <t>spp-125</t>
   </si>
   <si>
     <t>Januari</t>
   </si>
   <si>
-    <t>februari</t>
-  </si>
-  <si>
-    <t>maret</t>
-  </si>
-  <si>
-    <t>admin2</t>
-  </si>
-  <si>
     <t>Belum Lunas</t>
   </si>
   <si>
-    <t>lunas</t>
-  </si>
-  <si>
-    <t>spp-126</t>
-  </si>
-  <si>
-    <t>desember</t>
-  </si>
-  <si>
-    <t>Asti</t>
+    <t>2022-01-12</t>
+  </si>
+  <si>
+    <t>2022-01-14</t>
+  </si>
+  <si>
+    <t>Fadil</t>
   </si>
   <si>
     <t>Angga</t>
   </si>
   <si>
-    <t>Fadil</t>
-  </si>
-  <si>
-    <t>Fajar</t>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>SPP2</t>
+  </si>
+  <si>
+    <t>Maret</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>2022-01-16</t>
   </si>
 </sst>
 </file>
@@ -134,7 +137,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="yy/mm/dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,6 +148,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,28 +550,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -579,10 +588,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -606,189 +615,155 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>192010003</v>
+        <v>192010005</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J2" s="3">
-        <v>300000</v>
+        <v>250000</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="4">
-        <v>43842</v>
+        <v>17</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I3" s="1"/>
+      <c r="J3" s="3"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>192010004</v>
       </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>2020</v>
-      </c>
-      <c r="G3">
-        <v>2021</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="3">
-        <v>300000</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="4">
-        <v>43843</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>192010005</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="G4">
+        <v>2022</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="3">
+        <v>250000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>192010004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
         <v>2021</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="3">
-        <v>300000</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="G6">
+        <v>2022</v>
+      </c>
+      <c r="H6" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="4">
-        <v>43844</v>
-      </c>
-      <c r="N4" t="s">
-        <v>25</v>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="3">
+        <v>250000</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>192010006</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>2020</v>
-      </c>
-      <c r="G5">
-        <v>2021</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="3">
-        <v>300000</v>
-      </c>
-      <c r="K5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4">
-        <v>43845</v>
-      </c>
-      <c r="N5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M7" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
@@ -803,7 +778,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -815,7 +790,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>